<commit_message>
T4.1 update data extraction files and make overall data processing script
</commit_message>
<xml_diff>
--- a/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_Tsagarakis.xlsx
+++ b/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_Tsagarakis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://share.dtu.dk/sites/SEAwise_517900/Shared Documents/WP4 Ecological effects of fisheries/Task 4.1/Data extraction/Data extraction files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150CF4F4-0FE0-42CF-9AC8-577EBBCF87CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C64EF7D7-ADE5-4ACD-A4C3-35460CFA7B17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Drop-down overview" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DataExtraction!$A$2:$AX$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DataExtraction!$A$2:$AX$56</definedName>
     <definedName name="Benthic_epifauna">Validation!$AI$32:$AI$35</definedName>
     <definedName name="Benthos">Validation!$AN$24:$AN$25</definedName>
     <definedName name="Catch_and_bycatch">Validation!$AM$15:$AM$17</definedName>
@@ -2395,7 +2395,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2427" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2605" uniqueCount="470">
   <si>
     <t>SearchID</t>
   </si>
@@ -3708,9 +3708,6 @@
     <t>Spearman = −0.711;p &lt; 0.01</t>
   </si>
   <si>
-    <t>fishing presence</t>
-  </si>
-  <si>
     <t>fish size</t>
   </si>
   <si>
@@ -3805,6 +3802,9 @@
   </si>
   <si>
     <t>there was no difference in mean trophic level between the CIMR and the exploited areas</t>
+  </si>
+  <si>
+    <t>protected area</t>
   </si>
 </sst>
 </file>
@@ -3951,7 +3951,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3992,6 +3992,8 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4278,10 +4280,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AX51"/>
+  <dimension ref="A1:AX56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AX54" sqref="AX54"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AU62" sqref="AU62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6798,7 +6800,7 @@
         <v>207</v>
       </c>
       <c r="AX20" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="21" spans="1:50" x14ac:dyDescent="0.35">
@@ -8432,7 +8434,7 @@
         <v>161</v>
       </c>
       <c r="AO33" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="AQ33" t="s">
         <v>164</v>
@@ -8554,7 +8556,7 @@
         <v>161</v>
       </c>
       <c r="AO34" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="AQ34" t="s">
         <v>164</v>
@@ -8566,7 +8568,7 @@
         <v>189</v>
       </c>
       <c r="AU34" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="AV34" t="s">
         <v>200</v>
@@ -8670,7 +8672,7 @@
         <v>144</v>
       </c>
       <c r="AL35" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="AM35" t="s">
         <v>232</v>
@@ -8679,7 +8681,7 @@
         <v>161</v>
       </c>
       <c r="AO35" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="AQ35" t="s">
         <v>164</v>
@@ -8691,7 +8693,7 @@
         <v>189</v>
       </c>
       <c r="AU35" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="AV35" t="s">
         <v>200</v>
@@ -8700,7 +8702,7 @@
         <v>207</v>
       </c>
       <c r="AX35" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="36" spans="1:50" x14ac:dyDescent="0.35">
@@ -8798,7 +8800,7 @@
         <v>144</v>
       </c>
       <c r="AL36" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="AM36" t="s">
         <v>232</v>
@@ -8807,7 +8809,7 @@
         <v>161</v>
       </c>
       <c r="AO36" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="AQ36" t="s">
         <v>164</v>
@@ -8819,7 +8821,7 @@
         <v>189</v>
       </c>
       <c r="AU36" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="AV36" t="s">
         <v>200</v>
@@ -8828,7 +8830,7 @@
         <v>208</v>
       </c>
       <c r="AX36" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="37" spans="1:50" x14ac:dyDescent="0.35">
@@ -8932,7 +8934,7 @@
         <v>161</v>
       </c>
       <c r="AO37" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="AQ37" t="s">
         <v>164</v>
@@ -8944,7 +8946,7 @@
         <v>189</v>
       </c>
       <c r="AU37" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AV37" t="s">
         <v>205</v>
@@ -8953,7 +8955,7 @@
         <v>209</v>
       </c>
       <c r="AX37" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="38" spans="1:50" x14ac:dyDescent="0.35">
@@ -9057,7 +9059,7 @@
         <v>161</v>
       </c>
       <c r="AO38" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="AQ38" t="s">
         <v>164</v>
@@ -9069,7 +9071,7 @@
         <v>189</v>
       </c>
       <c r="AU38" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="AV38" t="s">
         <v>203</v>
@@ -9078,7 +9080,7 @@
         <v>210</v>
       </c>
       <c r="AX38" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="39" spans="1:50" x14ac:dyDescent="0.35">
@@ -9164,7 +9166,7 @@
         <v>3</v>
       </c>
       <c r="AD39" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="AF39" s="10" t="s">
         <v>253</v>
@@ -9176,13 +9178,13 @@
         <v>116</v>
       </c>
       <c r="AL39" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="AM39" t="s">
         <v>159</v>
       </c>
       <c r="AO39" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="AQ39" t="s">
         <v>164</v>
@@ -9194,7 +9196,7 @@
         <v>175</v>
       </c>
       <c r="AU39" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="AV39" t="s">
         <v>212</v>
@@ -9203,370 +9205,367 @@
         <v>210</v>
       </c>
     </row>
-    <row r="40" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A40" s="10" t="s">
+    <row r="40" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="18" t="s">
         <v>353</v>
       </c>
-      <c r="B40" s="10" t="s">
+      <c r="B40" s="18" t="s">
         <v>243</v>
       </c>
-      <c r="C40" s="10" t="s">
+      <c r="C40" s="18" t="s">
         <v>354</v>
       </c>
-      <c r="D40" s="10" t="s">
+      <c r="D40" s="18" t="s">
         <v>355</v>
       </c>
-      <c r="E40" s="10">
+      <c r="E40" s="18">
         <v>1998</v>
       </c>
-      <c r="F40" s="10" t="s">
+      <c r="F40" s="18" t="s">
         <v>356</v>
       </c>
-      <c r="G40" s="10" t="s">
+      <c r="G40" s="18" t="s">
         <v>357</v>
       </c>
-      <c r="H40" s="10" t="s">
+      <c r="H40" s="18" t="s">
         <v>320</v>
       </c>
-      <c r="I40" s="10" t="s">
+      <c r="I40" s="18" t="s">
         <v>358</v>
       </c>
-      <c r="J40" s="10" t="s">
+      <c r="J40" s="18" t="s">
         <v>359</v>
       </c>
-      <c r="K40" s="10" t="s">
+      <c r="K40" s="18" t="s">
         <v>360</v>
       </c>
-      <c r="L40" s="10" t="s">
+      <c r="L40" s="18" t="s">
         <v>248</v>
       </c>
-      <c r="M40" s="10" t="s">
+      <c r="M40" s="18" t="s">
         <v>361</v>
       </c>
-      <c r="N40" s="10" t="s">
+      <c r="N40" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="O40" s="10" t="s">
+      <c r="O40" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="P40" s="10" t="s">
+      <c r="P40" s="18" t="s">
         <v>275</v>
       </c>
-      <c r="Q40" s="10" t="s">
+      <c r="Q40" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="S40" t="s">
+      <c r="S40" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="T40" t="s">
+      <c r="T40" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="U40" t="s">
+      <c r="U40" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="V40" t="s">
+      <c r="V40" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="W40" t="s">
+      <c r="W40" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="X40" t="s">
+      <c r="X40" s="19" t="s">
         <v>215</v>
       </c>
-      <c r="Z40" t="s">
+      <c r="Z40" s="19" t="s">
+        <v>446</v>
+      </c>
+      <c r="AA40" s="19">
+        <v>2</v>
+      </c>
+      <c r="AB40" s="19">
+        <v>2</v>
+      </c>
+      <c r="AC40" s="19">
+        <v>3</v>
+      </c>
+      <c r="AF40" s="18" t="s">
+        <v>253</v>
+      </c>
+      <c r="AG40" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="AH40" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI40" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="AM40" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="AN40" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="AO40" s="19" t="s">
+        <v>469</v>
+      </c>
+      <c r="AQ40" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="AR40" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="AS40" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="AU40" s="19" t="s">
         <v>447</v>
       </c>
-      <c r="AA40">
+      <c r="AV40" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="AW40" s="19" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="41" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="B41" s="18" t="s">
+        <v>243</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="E41" s="18">
+        <v>1998</v>
+      </c>
+      <c r="F41" s="18" t="s">
+        <v>356</v>
+      </c>
+      <c r="G41" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="H41" s="18" t="s">
+        <v>320</v>
+      </c>
+      <c r="I41" s="18" t="s">
+        <v>358</v>
+      </c>
+      <c r="J41" s="18" t="s">
+        <v>359</v>
+      </c>
+      <c r="K41" s="18" t="s">
+        <v>360</v>
+      </c>
+      <c r="L41" s="18" t="s">
+        <v>248</v>
+      </c>
+      <c r="M41" s="18" t="s">
+        <v>361</v>
+      </c>
+      <c r="N41" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="O41" s="18" t="s">
+        <v>252</v>
+      </c>
+      <c r="P41" s="18" t="s">
+        <v>275</v>
+      </c>
+      <c r="Q41" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="S41" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="T41" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="U41" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="V41" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="W41" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="X41" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="Z41" s="19" t="s">
+        <v>446</v>
+      </c>
+      <c r="AA41" s="19">
         <v>2</v>
       </c>
-      <c r="AB40">
+      <c r="AB41" s="19">
         <v>2</v>
       </c>
-      <c r="AC40">
+      <c r="AC41" s="19">
         <v>3</v>
       </c>
-      <c r="AF40" s="10" t="s">
+      <c r="AF41" s="18" t="s">
         <v>253</v>
       </c>
-      <c r="AG40" t="s">
+      <c r="AG41" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="AH40" t="s">
+      <c r="AH41" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="AI40" t="s">
+      <c r="AI41" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="AM40" t="s">
+      <c r="AM41" s="19" t="s">
         <v>232</v>
       </c>
-      <c r="AN40" t="s">
-        <v>160</v>
-      </c>
-      <c r="AO40" t="s">
-        <v>437</v>
-      </c>
-      <c r="AQ40" t="s">
+      <c r="AN41" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="AO41" s="19" t="s">
+        <v>469</v>
+      </c>
+      <c r="AQ41" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="AR40" t="s">
+      <c r="AR41" s="19" t="s">
         <v>239</v>
       </c>
-      <c r="AS40" t="s">
+      <c r="AS41" s="19" t="s">
         <v>176</v>
       </c>
-      <c r="AU40" t="s">
-        <v>448</v>
-      </c>
-      <c r="AV40" t="s">
+      <c r="AU41" s="19" t="s">
+        <v>447</v>
+      </c>
+      <c r="AV41" s="19" t="s">
         <v>200</v>
       </c>
-      <c r="AW40" t="s">
-        <v>208</v>
+      <c r="AW41" s="19" t="s">
+        <v>210</v>
       </c>
     </row>
-    <row r="41" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A41" s="10" t="s">
+    <row r="42" spans="1:50" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="18" t="s">
         <v>353</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B42" s="18" t="s">
         <v>243</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C42" s="18" t="s">
         <v>354</v>
       </c>
-      <c r="D41" s="10" t="s">
+      <c r="D42" s="18" t="s">
         <v>355</v>
       </c>
-      <c r="E41" s="10">
+      <c r="E42" s="18">
         <v>1998</v>
       </c>
-      <c r="F41" s="10" t="s">
+      <c r="F42" s="18" t="s">
         <v>356</v>
       </c>
-      <c r="G41" s="10" t="s">
+      <c r="G42" s="18" t="s">
         <v>357</v>
       </c>
-      <c r="H41" s="10" t="s">
+      <c r="H42" s="18" t="s">
         <v>320</v>
       </c>
-      <c r="I41" s="10" t="s">
+      <c r="I42" s="18" t="s">
         <v>358</v>
       </c>
-      <c r="J41" s="10" t="s">
+      <c r="J42" s="18" t="s">
         <v>359</v>
       </c>
-      <c r="K41" s="10" t="s">
+      <c r="K42" s="18" t="s">
         <v>360</v>
       </c>
-      <c r="L41" s="10" t="s">
+      <c r="L42" s="18" t="s">
         <v>248</v>
       </c>
-      <c r="M41" s="10" t="s">
+      <c r="M42" s="18" t="s">
         <v>361</v>
       </c>
-      <c r="N41" s="10" t="s">
+      <c r="N42" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="O41" s="10" t="s">
+      <c r="O42" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="P41" s="10" t="s">
+      <c r="P42" s="18" t="s">
         <v>275</v>
       </c>
-      <c r="Q41" s="10" t="s">
+      <c r="Q42" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="S41" t="s">
+      <c r="S42" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="T41" t="s">
+      <c r="T42" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="U41" t="s">
+      <c r="U42" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="V41" t="s">
+      <c r="V42" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="W41" t="s">
+      <c r="W42" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="X41" t="s">
+      <c r="X42" s="19" t="s">
         <v>215</v>
       </c>
-      <c r="Z41" t="s">
+      <c r="Z42" s="19" t="s">
+        <v>446</v>
+      </c>
+      <c r="AA42" s="19">
+        <v>2</v>
+      </c>
+      <c r="AB42" s="19">
+        <v>2</v>
+      </c>
+      <c r="AC42" s="19">
+        <v>3</v>
+      </c>
+      <c r="AF42" s="18" t="s">
+        <v>253</v>
+      </c>
+      <c r="AG42" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="AH42" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="AM42" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="AN42" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="AO42" s="19" t="s">
+        <v>469</v>
+      </c>
+      <c r="AQ42" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="AR42" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="AS42" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="AU42" s="19" t="s">
         <v>447</v>
       </c>
-      <c r="AA41">
-        <v>2</v>
-      </c>
-      <c r="AB41">
-        <v>2</v>
-      </c>
-      <c r="AC41">
-        <v>3</v>
-      </c>
-      <c r="AF41" s="10" t="s">
-        <v>253</v>
-      </c>
-      <c r="AG41" t="s">
-        <v>110</v>
-      </c>
-      <c r="AH41" t="s">
-        <v>117</v>
-      </c>
-      <c r="AI41" t="s">
-        <v>144</v>
-      </c>
-      <c r="AM41" t="s">
-        <v>232</v>
-      </c>
-      <c r="AN41" t="s">
-        <v>161</v>
-      </c>
-      <c r="AO41" t="s">
-        <v>437</v>
-      </c>
-      <c r="AQ41" t="s">
-        <v>164</v>
-      </c>
-      <c r="AR41" t="s">
-        <v>239</v>
-      </c>
-      <c r="AS41" t="s">
-        <v>176</v>
-      </c>
-      <c r="AU41" t="s">
-        <v>429</v>
-      </c>
-      <c r="AV41" t="s">
-        <v>199</v>
-      </c>
-      <c r="AW41" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="42" spans="1:50" x14ac:dyDescent="0.35">
-      <c r="A42" s="10" t="s">
-        <v>353</v>
-      </c>
-      <c r="B42" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>354</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>355</v>
-      </c>
-      <c r="E42" s="10">
-        <v>1998</v>
-      </c>
-      <c r="F42" s="10" t="s">
-        <v>356</v>
-      </c>
-      <c r="G42" s="10" t="s">
-        <v>357</v>
-      </c>
-      <c r="H42" s="10" t="s">
-        <v>320</v>
-      </c>
-      <c r="I42" s="10" t="s">
-        <v>358</v>
-      </c>
-      <c r="J42" s="10" t="s">
-        <v>359</v>
-      </c>
-      <c r="K42" s="10" t="s">
-        <v>360</v>
-      </c>
-      <c r="L42" s="10" t="s">
-        <v>248</v>
-      </c>
-      <c r="M42" s="10" t="s">
-        <v>361</v>
-      </c>
-      <c r="N42" s="10" t="s">
-        <v>251</v>
-      </c>
-      <c r="O42" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="P42" s="10" t="s">
-        <v>275</v>
-      </c>
-      <c r="Q42" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="S42" t="s">
-        <v>24</v>
-      </c>
-      <c r="T42" t="s">
-        <v>46</v>
-      </c>
-      <c r="U42" t="s">
-        <v>58</v>
-      </c>
-      <c r="V42" t="s">
-        <v>44</v>
-      </c>
-      <c r="W42" t="s">
-        <v>55</v>
-      </c>
-      <c r="X42" t="s">
-        <v>215</v>
-      </c>
-      <c r="Z42" t="s">
-        <v>447</v>
-      </c>
-      <c r="AA42">
-        <v>2</v>
-      </c>
-      <c r="AB42">
-        <v>2</v>
-      </c>
-      <c r="AC42">
-        <v>3</v>
-      </c>
-      <c r="AF42" s="10" t="s">
-        <v>253</v>
-      </c>
-      <c r="AG42" t="s">
-        <v>110</v>
-      </c>
-      <c r="AH42" t="s">
-        <v>117</v>
-      </c>
-      <c r="AI42" t="s">
-        <v>144</v>
-      </c>
-      <c r="AM42" t="s">
-        <v>232</v>
-      </c>
-      <c r="AN42" t="s">
-        <v>160</v>
-      </c>
-      <c r="AO42" t="s">
-        <v>437</v>
-      </c>
-      <c r="AQ42" t="s">
-        <v>164</v>
-      </c>
-      <c r="AR42" t="s">
-        <v>239</v>
-      </c>
-      <c r="AS42" t="s">
-        <v>176</v>
-      </c>
-      <c r="AU42" t="s">
-        <v>429</v>
-      </c>
-      <c r="AV42" t="s">
-        <v>199</v>
-      </c>
-      <c r="AW42" t="s">
-        <v>208</v>
+      <c r="AV42" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="AW42" s="19" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="43" spans="1:50" x14ac:dyDescent="0.35">
@@ -9640,7 +9639,7 @@
         <v>215</v>
       </c>
       <c r="Z43" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="AA43">
         <v>2</v>
@@ -9658,16 +9657,19 @@
         <v>110</v>
       </c>
       <c r="AH43" t="s">
-        <v>124</v>
+        <v>117</v>
+      </c>
+      <c r="AI43" t="s">
+        <v>144</v>
       </c>
       <c r="AM43" t="s">
         <v>232</v>
       </c>
       <c r="AN43" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AO43" t="s">
-        <v>437</v>
+        <v>469</v>
       </c>
       <c r="AQ43" t="s">
         <v>164</v>
@@ -9679,54 +9681,54 @@
         <v>176</v>
       </c>
       <c r="AU43" t="s">
-        <v>449</v>
+        <v>429</v>
       </c>
       <c r="AV43" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="AW43" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="44" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A44" s="10" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="B44" s="10" t="s">
         <v>243</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="E44" s="10">
         <v>1998</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="H44" s="10" t="s">
-        <v>300</v>
+        <v>320</v>
       </c>
       <c r="I44" s="10" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="J44" s="10" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="K44" s="10" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="L44" s="10" t="s">
         <v>248</v>
       </c>
       <c r="M44" s="10" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
       <c r="N44" s="10" t="s">
         <v>251</v>
@@ -9735,31 +9737,31 @@
         <v>252</v>
       </c>
       <c r="P44" s="10" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
       <c r="Q44" s="10" t="s">
         <v>21</v>
       </c>
       <c r="S44" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="T44" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="U44" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="V44" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="W44" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="X44" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="Z44" t="s">
-        <v>405</v>
+        <v>446</v>
       </c>
       <c r="AA44">
         <v>2</v>
@@ -9770,32 +9772,23 @@
       <c r="AC44">
         <v>3</v>
       </c>
-      <c r="AD44" t="s">
-        <v>452</v>
-      </c>
       <c r="AF44" s="10" t="s">
         <v>253</v>
       </c>
       <c r="AG44" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="AH44" t="s">
-        <v>120</v>
-      </c>
-      <c r="AI44" t="s">
-        <v>140</v>
-      </c>
-      <c r="AJ44" t="s">
-        <v>113</v>
-      </c>
-      <c r="AL44" t="s">
-        <v>450</v>
+        <v>220</v>
       </c>
       <c r="AM44" t="s">
-        <v>159</v>
+        <v>232</v>
+      </c>
+      <c r="AN44" t="s">
+        <v>161</v>
       </c>
       <c r="AO44" t="s">
-        <v>451</v>
+        <v>469</v>
       </c>
       <c r="AQ44" t="s">
         <v>164</v>
@@ -9807,7 +9800,7 @@
         <v>176</v>
       </c>
       <c r="AU44" t="s">
-        <v>417</v>
+        <v>429</v>
       </c>
       <c r="AV44" t="s">
         <v>199</v>
@@ -9818,43 +9811,43 @@
     </row>
     <row r="45" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A45" s="10" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="B45" s="10" t="s">
         <v>243</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="E45" s="10">
         <v>1998</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="G45" s="10" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="H45" s="10" t="s">
-        <v>300</v>
+        <v>320</v>
       </c>
       <c r="I45" s="10" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="J45" s="10" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="K45" s="10" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="L45" s="10" t="s">
         <v>248</v>
       </c>
       <c r="M45" s="10" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
       <c r="N45" s="10" t="s">
         <v>251</v>
@@ -9863,31 +9856,31 @@
         <v>252</v>
       </c>
       <c r="P45" s="10" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
       <c r="Q45" s="10" t="s">
         <v>21</v>
       </c>
       <c r="S45" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="T45" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="U45" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="V45" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="W45" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="X45" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="Z45" t="s">
-        <v>405</v>
+        <v>446</v>
       </c>
       <c r="AA45">
         <v>2</v>
@@ -9898,35 +9891,26 @@
       <c r="AC45">
         <v>3</v>
       </c>
-      <c r="AD45" t="s">
-        <v>452</v>
-      </c>
       <c r="AF45" s="10" t="s">
         <v>253</v>
       </c>
       <c r="AG45" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="AH45" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="AI45" t="s">
-        <v>140</v>
-      </c>
-      <c r="AJ45" t="s">
-        <v>113</v>
-      </c>
-      <c r="AL45" t="s">
-        <v>453</v>
+        <v>144</v>
       </c>
       <c r="AM45" t="s">
         <v>232</v>
       </c>
       <c r="AN45" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AO45" t="s">
-        <v>451</v>
+        <v>469</v>
       </c>
       <c r="AQ45" t="s">
         <v>164</v>
@@ -9938,54 +9922,54 @@
         <v>176</v>
       </c>
       <c r="AU45" t="s">
-        <v>454</v>
+        <v>429</v>
       </c>
       <c r="AV45" t="s">
-        <v>238</v>
+        <v>199</v>
       </c>
       <c r="AW45" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="46" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A46" s="10" t="s">
-        <v>371</v>
+        <v>353</v>
       </c>
       <c r="B46" s="10" t="s">
         <v>243</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>372</v>
+        <v>354</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>373</v>
+        <v>355</v>
       </c>
       <c r="E46" s="10">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>374</v>
+        <v>356</v>
       </c>
       <c r="G46" s="10" t="s">
-        <v>340</v>
+        <v>357</v>
       </c>
       <c r="H46" s="10" t="s">
-        <v>300</v>
+        <v>320</v>
       </c>
       <c r="I46" s="10" t="s">
-        <v>301</v>
+        <v>358</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>375</v>
+        <v>359</v>
       </c>
       <c r="K46" s="10" t="s">
-        <v>248</v>
+        <v>360</v>
       </c>
       <c r="L46" s="10" t="s">
         <v>248</v>
       </c>
       <c r="M46" s="10" t="s">
-        <v>376</v>
+        <v>361</v>
       </c>
       <c r="N46" s="10" t="s">
         <v>251</v>
@@ -9994,31 +9978,31 @@
         <v>252</v>
       </c>
       <c r="P46" s="10" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
       <c r="Q46" s="10" t="s">
         <v>21</v>
       </c>
       <c r="S46" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="T46" t="s">
         <v>46</v>
       </c>
       <c r="U46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V46" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="W46" t="s">
         <v>55</v>
       </c>
       <c r="X46" t="s">
-        <v>69</v>
+        <v>215</v>
       </c>
       <c r="Z46" t="s">
-        <v>455</v>
+        <v>446</v>
       </c>
       <c r="AA46">
         <v>2</v>
@@ -10027,31 +10011,28 @@
         <v>2</v>
       </c>
       <c r="AC46">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF46" s="10" t="s">
-        <v>456</v>
+        <v>253</v>
       </c>
       <c r="AG46" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="AH46" t="s">
-        <v>220</v>
+        <v>117</v>
       </c>
       <c r="AI46" t="s">
-        <v>145</v>
-      </c>
-      <c r="AL46" t="s">
-        <v>457</v>
+        <v>144</v>
       </c>
       <c r="AM46" t="s">
         <v>232</v>
       </c>
       <c r="AN46" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="AO46" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
       <c r="AQ46" t="s">
         <v>164</v>
@@ -10060,57 +10041,57 @@
         <v>239</v>
       </c>
       <c r="AS46" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AU46" t="s">
-        <v>417</v>
+        <v>448</v>
       </c>
       <c r="AV46" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="AW46" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="47" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A47" s="10" t="s">
-        <v>371</v>
+        <v>353</v>
       </c>
       <c r="B47" s="10" t="s">
         <v>243</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>372</v>
+        <v>354</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>373</v>
+        <v>355</v>
       </c>
       <c r="E47" s="10">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>374</v>
+        <v>356</v>
       </c>
       <c r="G47" s="10" t="s">
-        <v>340</v>
+        <v>357</v>
       </c>
       <c r="H47" s="10" t="s">
-        <v>300</v>
+        <v>320</v>
       </c>
       <c r="I47" s="10" t="s">
-        <v>301</v>
+        <v>358</v>
       </c>
       <c r="J47" s="10" t="s">
-        <v>375</v>
+        <v>359</v>
       </c>
       <c r="K47" s="10" t="s">
-        <v>248</v>
+        <v>360</v>
       </c>
       <c r="L47" s="10" t="s">
         <v>248</v>
       </c>
       <c r="M47" s="10" t="s">
-        <v>376</v>
+        <v>361</v>
       </c>
       <c r="N47" s="10" t="s">
         <v>251</v>
@@ -10119,31 +10100,31 @@
         <v>252</v>
       </c>
       <c r="P47" s="10" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
       <c r="Q47" s="10" t="s">
         <v>21</v>
       </c>
       <c r="S47" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="T47" t="s">
         <v>46</v>
       </c>
       <c r="U47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V47" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="W47" t="s">
         <v>55</v>
       </c>
       <c r="X47" t="s">
-        <v>69</v>
+        <v>215</v>
       </c>
       <c r="Z47" t="s">
-        <v>455</v>
+        <v>446</v>
       </c>
       <c r="AA47">
         <v>2</v>
@@ -10152,31 +10133,28 @@
         <v>2</v>
       </c>
       <c r="AC47">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF47" s="10" t="s">
-        <v>456</v>
+        <v>253</v>
       </c>
       <c r="AG47" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="AH47" t="s">
-        <v>220</v>
+        <v>117</v>
       </c>
       <c r="AI47" t="s">
-        <v>145</v>
-      </c>
-      <c r="AL47" t="s">
-        <v>459</v>
+        <v>144</v>
       </c>
       <c r="AM47" t="s">
         <v>232</v>
       </c>
       <c r="AN47" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AO47" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
       <c r="AQ47" t="s">
         <v>164</v>
@@ -10185,13 +10163,13 @@
         <v>239</v>
       </c>
       <c r="AS47" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AU47" t="s">
-        <v>417</v>
+        <v>448</v>
       </c>
       <c r="AV47" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="AW47" t="s">
         <v>210</v>
@@ -10199,43 +10177,43 @@
     </row>
     <row r="48" spans="1:50" x14ac:dyDescent="0.35">
       <c r="A48" s="10" t="s">
-        <v>371</v>
+        <v>353</v>
       </c>
       <c r="B48" s="10" t="s">
         <v>243</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>372</v>
+        <v>354</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>373</v>
+        <v>355</v>
       </c>
       <c r="E48" s="10">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="F48" s="10" t="s">
-        <v>374</v>
+        <v>356</v>
       </c>
       <c r="G48" s="10" t="s">
-        <v>340</v>
+        <v>357</v>
       </c>
       <c r="H48" s="10" t="s">
-        <v>300</v>
+        <v>320</v>
       </c>
       <c r="I48" s="10" t="s">
-        <v>301</v>
+        <v>358</v>
       </c>
       <c r="J48" s="10" t="s">
-        <v>375</v>
+        <v>359</v>
       </c>
       <c r="K48" s="10" t="s">
-        <v>248</v>
+        <v>360</v>
       </c>
       <c r="L48" s="10" t="s">
         <v>248</v>
       </c>
       <c r="M48" s="10" t="s">
-        <v>376</v>
+        <v>361</v>
       </c>
       <c r="N48" s="10" t="s">
         <v>251</v>
@@ -10244,31 +10222,31 @@
         <v>252</v>
       </c>
       <c r="P48" s="10" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
       <c r="Q48" s="10" t="s">
         <v>21</v>
       </c>
       <c r="S48" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="T48" t="s">
         <v>46</v>
       </c>
       <c r="U48" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V48" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="W48" t="s">
         <v>55</v>
       </c>
       <c r="X48" t="s">
-        <v>69</v>
+        <v>215</v>
       </c>
       <c r="Z48" t="s">
-        <v>455</v>
+        <v>446</v>
       </c>
       <c r="AA48">
         <v>2</v>
@@ -10277,31 +10255,25 @@
         <v>2</v>
       </c>
       <c r="AC48">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF48" s="10" t="s">
-        <v>456</v>
+        <v>253</v>
       </c>
       <c r="AG48" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="AH48" t="s">
         <v>220</v>
       </c>
-      <c r="AI48" t="s">
-        <v>139</v>
-      </c>
-      <c r="AL48" t="s">
-        <v>460</v>
-      </c>
       <c r="AM48" t="s">
         <v>232</v>
       </c>
       <c r="AN48" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AO48" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
       <c r="AQ48" t="s">
         <v>164</v>
@@ -10310,13 +10282,13 @@
         <v>239</v>
       </c>
       <c r="AS48" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AU48" t="s">
-        <v>417</v>
+        <v>448</v>
       </c>
       <c r="AV48" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="AW48" t="s">
         <v>210</v>
@@ -10324,43 +10296,43 @@
     </row>
     <row r="49" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A49" s="10" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="B49" s="10" t="s">
         <v>243</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="E49" s="10">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="F49" s="10" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>340</v>
+        <v>366</v>
       </c>
       <c r="H49" s="10" t="s">
         <v>300</v>
       </c>
       <c r="I49" s="10" t="s">
-        <v>301</v>
+        <v>367</v>
       </c>
       <c r="J49" s="10" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="K49" s="10" t="s">
-        <v>248</v>
+        <v>369</v>
       </c>
       <c r="L49" s="10" t="s">
         <v>248</v>
       </c>
       <c r="M49" s="10" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="N49" s="10" t="s">
         <v>251</v>
@@ -10375,25 +10347,25 @@
         <v>21</v>
       </c>
       <c r="S49" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="T49" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="U49" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="V49" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="W49" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="X49" t="s">
-        <v>69</v>
+        <v>216</v>
       </c>
       <c r="Z49" t="s">
-        <v>455</v>
+        <v>405</v>
       </c>
       <c r="AA49">
         <v>2</v>
@@ -10402,31 +10374,34 @@
         <v>2</v>
       </c>
       <c r="AC49">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="AD49" t="s">
+        <v>451</v>
       </c>
       <c r="AF49" s="10" t="s">
-        <v>456</v>
+        <v>253</v>
       </c>
       <c r="AG49" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="AH49" t="s">
-        <v>220</v>
+        <v>120</v>
       </c>
       <c r="AI49" t="s">
-        <v>139</v>
+        <v>140</v>
+      </c>
+      <c r="AJ49" t="s">
+        <v>113</v>
       </c>
       <c r="AL49" t="s">
-        <v>461</v>
+        <v>449</v>
       </c>
       <c r="AM49" t="s">
-        <v>232</v>
-      </c>
-      <c r="AN49" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="AO49" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="AQ49" t="s">
         <v>164</v>
@@ -10435,7 +10410,7 @@
         <v>239</v>
       </c>
       <c r="AS49" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AU49" t="s">
         <v>417</v>
@@ -10444,48 +10419,48 @@
         <v>199</v>
       </c>
       <c r="AW49" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="50" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A50" s="10" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="B50" s="10" t="s">
         <v>243</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="E50" s="10">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>340</v>
+        <v>366</v>
       </c>
       <c r="H50" s="10" t="s">
         <v>300</v>
       </c>
       <c r="I50" s="10" t="s">
-        <v>301</v>
+        <v>367</v>
       </c>
       <c r="J50" s="10" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="K50" s="10" t="s">
-        <v>248</v>
+        <v>369</v>
       </c>
       <c r="L50" s="10" t="s">
         <v>248</v>
       </c>
       <c r="M50" s="10" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="N50" s="10" t="s">
         <v>251</v>
@@ -10500,25 +10475,25 @@
         <v>21</v>
       </c>
       <c r="S50" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="T50" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="U50" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="V50" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="W50" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="X50" t="s">
-        <v>69</v>
+        <v>216</v>
       </c>
       <c r="Z50" t="s">
-        <v>455</v>
+        <v>405</v>
       </c>
       <c r="AA50">
         <v>2</v>
@@ -10527,31 +10502,37 @@
         <v>2</v>
       </c>
       <c r="AC50">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="AD50" t="s">
+        <v>451</v>
       </c>
       <c r="AF50" s="10" t="s">
-        <v>456</v>
+        <v>253</v>
       </c>
       <c r="AG50" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="AH50" t="s">
-        <v>220</v>
+        <v>120</v>
       </c>
       <c r="AI50" t="s">
-        <v>131</v>
+        <v>140</v>
+      </c>
+      <c r="AJ50" t="s">
+        <v>113</v>
       </c>
       <c r="AL50" t="s">
-        <v>462</v>
+        <v>452</v>
       </c>
       <c r="AM50" t="s">
         <v>232</v>
       </c>
       <c r="AN50" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AO50" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="AQ50" t="s">
         <v>164</v>
@@ -10560,16 +10541,16 @@
         <v>239</v>
       </c>
       <c r="AS50" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AU50" t="s">
-        <v>417</v>
+        <v>453</v>
       </c>
       <c r="AV50" t="s">
-        <v>199</v>
+        <v>238</v>
       </c>
       <c r="AW50" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="51" spans="1:49" x14ac:dyDescent="0.35">
@@ -10643,7 +10624,7 @@
         <v>69</v>
       </c>
       <c r="Z51" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="AA51">
         <v>2</v>
@@ -10655,28 +10636,28 @@
         <v>2</v>
       </c>
       <c r="AF51" s="10" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="AG51" t="s">
         <v>109</v>
       </c>
       <c r="AH51" t="s">
-        <v>117</v>
+        <v>220</v>
       </c>
       <c r="AI51" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AL51" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="AM51" t="s">
         <v>232</v>
       </c>
       <c r="AN51" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="AO51" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="AQ51" t="s">
         <v>164</v>
@@ -10694,6 +10675,631 @@
         <v>199</v>
       </c>
       <c r="AW51" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="52" spans="1:49" x14ac:dyDescent="0.35">
+      <c r="A52" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>372</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="E52" s="10">
+        <v>1997</v>
+      </c>
+      <c r="F52" s="10" t="s">
+        <v>374</v>
+      </c>
+      <c r="G52" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="H52" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="I52" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="J52" s="10" t="s">
+        <v>375</v>
+      </c>
+      <c r="K52" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="L52" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="M52" s="10" t="s">
+        <v>376</v>
+      </c>
+      <c r="N52" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="O52" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="P52" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q52" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="S52" t="s">
+        <v>31</v>
+      </c>
+      <c r="T52" t="s">
+        <v>46</v>
+      </c>
+      <c r="U52" t="s">
+        <v>59</v>
+      </c>
+      <c r="V52" t="s">
+        <v>46</v>
+      </c>
+      <c r="W52" t="s">
+        <v>55</v>
+      </c>
+      <c r="X52" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z52" t="s">
+        <v>454</v>
+      </c>
+      <c r="AA52">
+        <v>2</v>
+      </c>
+      <c r="AB52">
+        <v>2</v>
+      </c>
+      <c r="AC52">
+        <v>2</v>
+      </c>
+      <c r="AF52" s="10" t="s">
+        <v>455</v>
+      </c>
+      <c r="AG52" t="s">
+        <v>109</v>
+      </c>
+      <c r="AH52" t="s">
+        <v>220</v>
+      </c>
+      <c r="AI52" t="s">
+        <v>145</v>
+      </c>
+      <c r="AL52" t="s">
+        <v>458</v>
+      </c>
+      <c r="AM52" t="s">
+        <v>232</v>
+      </c>
+      <c r="AN52" t="s">
+        <v>162</v>
+      </c>
+      <c r="AO52" t="s">
+        <v>457</v>
+      </c>
+      <c r="AQ52" t="s">
+        <v>164</v>
+      </c>
+      <c r="AR52" t="s">
+        <v>239</v>
+      </c>
+      <c r="AS52" t="s">
+        <v>175</v>
+      </c>
+      <c r="AU52" t="s">
+        <v>417</v>
+      </c>
+      <c r="AV52" t="s">
+        <v>199</v>
+      </c>
+      <c r="AW52" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="53" spans="1:49" x14ac:dyDescent="0.35">
+      <c r="A53" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>372</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="E53" s="10">
+        <v>1997</v>
+      </c>
+      <c r="F53" s="10" t="s">
+        <v>374</v>
+      </c>
+      <c r="G53" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="H53" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="I53" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="J53" s="10" t="s">
+        <v>375</v>
+      </c>
+      <c r="K53" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="L53" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="M53" s="10" t="s">
+        <v>376</v>
+      </c>
+      <c r="N53" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="O53" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="P53" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q53" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="S53" t="s">
+        <v>31</v>
+      </c>
+      <c r="T53" t="s">
+        <v>46</v>
+      </c>
+      <c r="U53" t="s">
+        <v>59</v>
+      </c>
+      <c r="V53" t="s">
+        <v>46</v>
+      </c>
+      <c r="W53" t="s">
+        <v>55</v>
+      </c>
+      <c r="X53" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z53" t="s">
+        <v>454</v>
+      </c>
+      <c r="AA53">
+        <v>2</v>
+      </c>
+      <c r="AB53">
+        <v>2</v>
+      </c>
+      <c r="AC53">
+        <v>2</v>
+      </c>
+      <c r="AF53" s="10" t="s">
+        <v>455</v>
+      </c>
+      <c r="AG53" t="s">
+        <v>109</v>
+      </c>
+      <c r="AH53" t="s">
+        <v>220</v>
+      </c>
+      <c r="AI53" t="s">
+        <v>139</v>
+      </c>
+      <c r="AL53" t="s">
+        <v>459</v>
+      </c>
+      <c r="AM53" t="s">
+        <v>232</v>
+      </c>
+      <c r="AN53" t="s">
+        <v>162</v>
+      </c>
+      <c r="AO53" t="s">
+        <v>457</v>
+      </c>
+      <c r="AQ53" t="s">
+        <v>164</v>
+      </c>
+      <c r="AR53" t="s">
+        <v>239</v>
+      </c>
+      <c r="AS53" t="s">
+        <v>175</v>
+      </c>
+      <c r="AU53" t="s">
+        <v>417</v>
+      </c>
+      <c r="AV53" t="s">
+        <v>199</v>
+      </c>
+      <c r="AW53" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="54" spans="1:49" x14ac:dyDescent="0.35">
+      <c r="A54" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>372</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="E54" s="10">
+        <v>1997</v>
+      </c>
+      <c r="F54" s="10" t="s">
+        <v>374</v>
+      </c>
+      <c r="G54" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="H54" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="I54" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="J54" s="10" t="s">
+        <v>375</v>
+      </c>
+      <c r="K54" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="L54" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="M54" s="10" t="s">
+        <v>376</v>
+      </c>
+      <c r="N54" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="O54" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="P54" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q54" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="S54" t="s">
+        <v>31</v>
+      </c>
+      <c r="T54" t="s">
+        <v>46</v>
+      </c>
+      <c r="U54" t="s">
+        <v>59</v>
+      </c>
+      <c r="V54" t="s">
+        <v>46</v>
+      </c>
+      <c r="W54" t="s">
+        <v>55</v>
+      </c>
+      <c r="X54" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z54" t="s">
+        <v>454</v>
+      </c>
+      <c r="AA54">
+        <v>2</v>
+      </c>
+      <c r="AB54">
+        <v>2</v>
+      </c>
+      <c r="AC54">
+        <v>2</v>
+      </c>
+      <c r="AF54" s="10" t="s">
+        <v>455</v>
+      </c>
+      <c r="AG54" t="s">
+        <v>109</v>
+      </c>
+      <c r="AH54" t="s">
+        <v>220</v>
+      </c>
+      <c r="AI54" t="s">
+        <v>139</v>
+      </c>
+      <c r="AL54" t="s">
+        <v>460</v>
+      </c>
+      <c r="AM54" t="s">
+        <v>232</v>
+      </c>
+      <c r="AN54" t="s">
+        <v>162</v>
+      </c>
+      <c r="AO54" t="s">
+        <v>457</v>
+      </c>
+      <c r="AQ54" t="s">
+        <v>164</v>
+      </c>
+      <c r="AR54" t="s">
+        <v>239</v>
+      </c>
+      <c r="AS54" t="s">
+        <v>175</v>
+      </c>
+      <c r="AU54" t="s">
+        <v>417</v>
+      </c>
+      <c r="AV54" t="s">
+        <v>199</v>
+      </c>
+      <c r="AW54" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="55" spans="1:49" x14ac:dyDescent="0.35">
+      <c r="A55" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>372</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="E55" s="10">
+        <v>1997</v>
+      </c>
+      <c r="F55" s="10" t="s">
+        <v>374</v>
+      </c>
+      <c r="G55" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="H55" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="I55" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="J55" s="10" t="s">
+        <v>375</v>
+      </c>
+      <c r="K55" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="L55" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="M55" s="10" t="s">
+        <v>376</v>
+      </c>
+      <c r="N55" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="O55" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="P55" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q55" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="S55" t="s">
+        <v>31</v>
+      </c>
+      <c r="T55" t="s">
+        <v>46</v>
+      </c>
+      <c r="U55" t="s">
+        <v>59</v>
+      </c>
+      <c r="V55" t="s">
+        <v>46</v>
+      </c>
+      <c r="W55" t="s">
+        <v>55</v>
+      </c>
+      <c r="X55" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z55" t="s">
+        <v>454</v>
+      </c>
+      <c r="AA55">
+        <v>2</v>
+      </c>
+      <c r="AB55">
+        <v>2</v>
+      </c>
+      <c r="AC55">
+        <v>2</v>
+      </c>
+      <c r="AF55" s="10" t="s">
+        <v>455</v>
+      </c>
+      <c r="AG55" t="s">
+        <v>109</v>
+      </c>
+      <c r="AH55" t="s">
+        <v>220</v>
+      </c>
+      <c r="AI55" t="s">
+        <v>131</v>
+      </c>
+      <c r="AL55" t="s">
+        <v>461</v>
+      </c>
+      <c r="AM55" t="s">
+        <v>232</v>
+      </c>
+      <c r="AN55" t="s">
+        <v>162</v>
+      </c>
+      <c r="AO55" t="s">
+        <v>457</v>
+      </c>
+      <c r="AQ55" t="s">
+        <v>164</v>
+      </c>
+      <c r="AR55" t="s">
+        <v>239</v>
+      </c>
+      <c r="AS55" t="s">
+        <v>175</v>
+      </c>
+      <c r="AU55" t="s">
+        <v>417</v>
+      </c>
+      <c r="AV55" t="s">
+        <v>199</v>
+      </c>
+      <c r="AW55" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="56" spans="1:49" x14ac:dyDescent="0.35">
+      <c r="A56" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>372</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="E56" s="10">
+        <v>1997</v>
+      </c>
+      <c r="F56" s="10" t="s">
+        <v>374</v>
+      </c>
+      <c r="G56" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="H56" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="I56" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="J56" s="10" t="s">
+        <v>375</v>
+      </c>
+      <c r="K56" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="L56" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="M56" s="10" t="s">
+        <v>376</v>
+      </c>
+      <c r="N56" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="O56" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="P56" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q56" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="S56" t="s">
+        <v>31</v>
+      </c>
+      <c r="T56" t="s">
+        <v>46</v>
+      </c>
+      <c r="U56" t="s">
+        <v>59</v>
+      </c>
+      <c r="V56" t="s">
+        <v>46</v>
+      </c>
+      <c r="W56" t="s">
+        <v>55</v>
+      </c>
+      <c r="X56" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z56" t="s">
+        <v>454</v>
+      </c>
+      <c r="AA56">
+        <v>2</v>
+      </c>
+      <c r="AB56">
+        <v>2</v>
+      </c>
+      <c r="AC56">
+        <v>2</v>
+      </c>
+      <c r="AF56" s="10" t="s">
+        <v>455</v>
+      </c>
+      <c r="AG56" t="s">
+        <v>109</v>
+      </c>
+      <c r="AH56" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI56" t="s">
+        <v>144</v>
+      </c>
+      <c r="AL56" t="s">
+        <v>462</v>
+      </c>
+      <c r="AM56" t="s">
+        <v>232</v>
+      </c>
+      <c r="AN56" t="s">
+        <v>160</v>
+      </c>
+      <c r="AO56" t="s">
+        <v>457</v>
+      </c>
+      <c r="AQ56" t="s">
+        <v>164</v>
+      </c>
+      <c r="AR56" t="s">
+        <v>239</v>
+      </c>
+      <c r="AS56" t="s">
+        <v>175</v>
+      </c>
+      <c r="AU56" t="s">
+        <v>417</v>
+      </c>
+      <c r="AV56" t="s">
+        <v>199</v>
+      </c>
+      <c r="AW56" t="s">
         <v>209</v>
       </c>
     </row>
@@ -10715,7 +11321,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ3:AQ1048576" xr:uid="{5FFD7ACF-9A7A-47E4-8F02-C092CA18B67C}">
       <formula1>Fishery_type</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI3:AJ1048576 AR3:AS1048576 AN3:AN1048576" xr:uid="{E3465DE4-B915-4C62-9316-EABEC40DC1E6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN3:AN1048576 AR3:AS1048576 AI3:AJ1048576" xr:uid="{E3465DE4-B915-4C62-9316-EABEC40DC1E6}">
       <formula1>INDIRECT(AH3)</formula1>
     </dataValidation>
   </dataValidations>
@@ -12808,12 +13414,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12931,15 +13534,25 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66D459FE-C8DA-484C-BC8E-5EB6A351EBC9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{495201D0-9695-4A45-BC3A-28D949F46F55}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -12961,16 +13574,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{495201D0-9695-4A45-BC3A-28D949F46F55}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66D459FE-C8DA-484C-BC8E-5EB6A351EBC9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>